<commit_message>
added binary for entail3
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luigi\Desktop\ENTAIL\fibrille\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1309F09C-7DA9-464E-A826-E9FF766307B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{44BB0010-F794-496C-BE06-4495D81785A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="45">
   <si>
     <t>VALIDATION</t>
   </si>
@@ -54,6 +54,9 @@
     <t>ValidationValue</t>
   </si>
   <si>
+    <t>Classificator configuration</t>
+  </si>
+  <si>
     <t>PCA</t>
   </si>
   <si>
@@ -75,70 +78,76 @@
     <t>AUC</t>
   </si>
   <si>
+    <t>SP (TNR)</t>
+  </si>
+  <si>
+    <t>SN (TPR)</t>
+  </si>
+  <si>
+    <t>FDR</t>
+  </si>
+  <si>
     <t xml:space="preserve">AUC </t>
   </si>
   <si>
+    <t>Cross Validation</t>
+  </si>
+  <si>
+    <t>Esemble; GentleBoost; Max Split 26; Num Learners 167; Learning Rate 0.5915</t>
+  </si>
+  <si>
     <t>NO</t>
   </si>
   <si>
+    <t>0.876</t>
+  </si>
+  <si>
+    <t>0.94</t>
+  </si>
+  <si>
+    <t>0.788</t>
+  </si>
+  <si>
+    <t>0.88</t>
+  </si>
+  <si>
+    <t>Naive Bayers;  Kernel Naive Bayes; Gaussian Kernel Type; Unbounded Support</t>
+  </si>
+  <si>
+    <t>0.814</t>
+  </si>
+  <si>
+    <t>0.82</t>
+  </si>
+  <si>
     <t>0.818</t>
   </si>
   <si>
+    <t>0.83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please note: There was not possible to identify a good classificator (accuracy &gt; 0.75) by using PCA. </t>
+  </si>
+  <si>
+    <t>Esemble; GentleBoost; Max Split 22; Num Learners auto; Learning Rate 0.00117855388820037</t>
+  </si>
+  <si>
+    <t>0.881</t>
+  </si>
+  <si>
+    <t>0.95</t>
+  </si>
+  <si>
+    <t>0.773</t>
+  </si>
+  <si>
+    <t>Esemble; GentleBoost; Max Split 40; Num Learners 80; Learning Rate 0.1</t>
+  </si>
+  <si>
+    <t>0.866</t>
+  </si>
+  <si>
     <t>0.89</t>
-  </si>
-  <si>
-    <t>0.83</t>
-  </si>
-  <si>
-    <t>0.82</t>
-  </si>
-  <si>
-    <t>Cross Validation</t>
-  </si>
-  <si>
-    <t>Classificator configuration</t>
-  </si>
-  <si>
-    <t>Esemble; GentleBoost; Max Split 26; Num Learners 167; Learning Rate 0.5915</t>
-  </si>
-  <si>
-    <t>0.876</t>
-  </si>
-  <si>
-    <t>0.94</t>
-  </si>
-  <si>
-    <t>0.88</t>
-  </si>
-  <si>
-    <t>0.788</t>
-  </si>
-  <si>
-    <t>Naive Bayers;  Kernel Naive Bayes; Gaussian Kernel Type; Unbounded Support</t>
-  </si>
-  <si>
-    <t>0.814</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please note: There was not possible to identify a good classificator (accuracy &gt; 0.75) by using PCA. </t>
-  </si>
-  <si>
-    <t>Esemble; GentleBoost; Max Split 22; Num Learners auto; Learning Rate 0.00117855388820037</t>
-  </si>
-  <si>
-    <t>0.881</t>
-  </si>
-  <si>
-    <t>0.95</t>
-  </si>
-  <si>
-    <t>0.773</t>
-  </si>
-  <si>
-    <t>0.866</t>
-  </si>
-  <si>
-    <t>Esemble; GentleBoost; Max Split 40; Num Learners 80; Learning Rate 0.1</t>
   </si>
   <si>
     <t>0.817</t>
@@ -273,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -290,12 +299,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -304,24 +307,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -603,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:R14"/>
+  <dimension ref="A2:X14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,30 +617,36 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" customWidth="1"/>
     <col min="7" max="7" width="20.140625" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G2" s="12" t="s">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="7" t="s">
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -651,49 +660,67 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="H3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="I3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="J3" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="K3" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="L3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="T3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>13</v>
+      <c r="U3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -701,55 +728,79 @@
         <v>4125</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4">
         <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" s="2">
+        <v>309</v>
+      </c>
+      <c r="I4" s="2">
+        <v>41</v>
+      </c>
+      <c r="J4" s="2">
+        <v>46</v>
+      </c>
+      <c r="K4" s="2">
+        <v>304</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="2">
+        <f>K4/SUM(K4,I4)</f>
+        <v>0.88115942028985506</v>
+      </c>
+      <c r="N4" s="2">
+        <f>H4/SUM(H4,J4)</f>
+        <v>0.87042253521126756</v>
+      </c>
+      <c r="O4" s="2">
+        <f>I4/SUM(I4,H4)</f>
+        <v>0.11714285714285715</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>19</v>
+      </c>
+      <c r="R4" s="2">
         <v>14</v>
       </c>
-      <c r="G4" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="14">
-        <v>309</v>
-      </c>
-      <c r="I4" s="14">
-        <v>41</v>
-      </c>
-      <c r="J4" s="14">
-        <v>46</v>
-      </c>
-      <c r="K4" s="14">
-        <v>304</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N4" s="2">
-        <v>19</v>
-      </c>
-      <c r="O4" s="2">
-        <v>14</v>
-      </c>
-      <c r="P4" s="2">
+      <c r="S4" s="2">
         <v>0</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="T4" s="2">
         <v>33</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="U4" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="V4">
+        <f>T4/SUM(T4,R4)</f>
+        <v>0.7021276595744681</v>
+      </c>
+      <c r="W4">
+        <f>Q4/SUM(Q4,S4)</f>
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <f>R4/SUM(R4,Q4)</f>
+        <v>0.42424242424242425</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -757,77 +808,104 @@
         <v>4125</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>5</v>
       </c>
       <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="14" t="s">
+      <c r="H5" s="2">
+        <v>261</v>
+      </c>
+      <c r="I5" s="2">
+        <v>89</v>
+      </c>
+      <c r="J5" s="2">
+        <v>41</v>
+      </c>
+      <c r="K5" s="2">
+        <v>309</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="14">
-        <v>261</v>
-      </c>
-      <c r="I5" s="14">
-        <v>89</v>
-      </c>
-      <c r="J5" s="14">
-        <v>41</v>
-      </c>
-      <c r="K5" s="14">
-        <v>309</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>15</v>
+      <c r="M5" s="2">
+        <f t="shared" ref="M5:M13" si="0">K5/SUM(K5,I5)</f>
+        <v>0.77638190954773867</v>
       </c>
       <c r="N5" s="2">
+        <f t="shared" ref="N5:N13" si="1">H5/SUM(H5,J5)</f>
+        <v>0.86423841059602646</v>
+      </c>
+      <c r="O5" s="2">
+        <f t="shared" ref="O5:O13" si="2">I5/SUM(I5,H5)</f>
+        <v>0.25428571428571428</v>
+      </c>
+      <c r="P5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5" s="2">
         <v>21</v>
       </c>
-      <c r="O5" s="2">
+      <c r="R5" s="2">
         <v>12</v>
       </c>
-      <c r="P5" s="2">
+      <c r="S5" s="2">
         <v>0</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="T5" s="2">
         <v>33</v>
       </c>
-      <c r="R5" s="2" t="s">
-        <v>17</v>
+      <c r="U5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="V5">
+        <f t="shared" ref="V5:V13" si="3">T5/SUM(T5,R5)</f>
+        <v>0.73333333333333328</v>
+      </c>
+      <c r="W5">
+        <f t="shared" ref="W5:W13" si="4">Q5/SUM(Q5,S5)</f>
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <f t="shared" ref="X5:X13" si="5">R5/SUM(R5,Q5)</f>
+        <v>0.36363636363636365</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
     </row>
-    <row r="7" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -835,55 +913,79 @@
         <v>4125</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7">
         <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="2">
+        <v>316</v>
+      </c>
+      <c r="I7" s="2">
+        <v>34</v>
+      </c>
+      <c r="J7" s="2">
+        <v>49</v>
+      </c>
+      <c r="K7" s="2">
+        <v>301</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.89850746268656712</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" si="1"/>
+        <v>0.86575342465753424</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" si="2"/>
+        <v>9.7142857142857142E-2</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>19</v>
+      </c>
+      <c r="R7" s="2">
         <v>14</v>
       </c>
-      <c r="G7" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="14">
-        <v>316</v>
-      </c>
-      <c r="I7" s="14">
-        <v>34</v>
-      </c>
-      <c r="J7" s="14">
-        <v>49</v>
-      </c>
-      <c r="K7" s="14">
-        <v>301</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M7" s="2" t="s">
+      <c r="S7" s="2">
+        <v>1</v>
+      </c>
+      <c r="T7" s="2">
         <v>32</v>
       </c>
-      <c r="N7" s="2">
-        <v>19</v>
-      </c>
-      <c r="O7" s="2">
-        <v>14</v>
-      </c>
-      <c r="P7" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>32</v>
-      </c>
-      <c r="R7" s="2" t="s">
+      <c r="U7" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="V7">
+        <f t="shared" si="3"/>
+        <v>0.69565217391304346</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="4"/>
+        <v>0.95</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="5"/>
+        <v>0.42424242424242425</v>
+      </c>
     </row>
-    <row r="8" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" ht="45" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -891,55 +993,79 @@
         <v>4125</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8">
         <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="14">
+        <v>20</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="2">
         <v>308</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="2">
         <v>42</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="2">
         <v>52</v>
       </c>
-      <c r="K8" s="14">
+      <c r="K8" s="2">
         <v>298</v>
       </c>
       <c r="L8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.87647058823529411</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.85555555555555551</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" si="2"/>
+        <v>0.12</v>
+      </c>
+      <c r="P8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N8" s="2">
+      <c r="Q8" s="2">
         <v>20</v>
       </c>
-      <c r="O8" s="2">
+      <c r="R8" s="2">
         <v>13</v>
       </c>
-      <c r="P8" s="2">
+      <c r="S8" s="2">
         <v>1</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="T8" s="2">
         <v>32</v>
       </c>
-      <c r="R8" s="2" t="s">
-        <v>16</v>
+      <c r="U8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="3"/>
+        <v>0.71111111111111114</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="4"/>
+        <v>0.95238095238095233</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="5"/>
+        <v>0.39393939393939392</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -947,189 +1073,264 @@
         <v>4125</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9">
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" s="14">
+        <v>20</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="2">
         <v>263</v>
       </c>
-      <c r="I9" s="14">
+      <c r="I9" s="2">
         <v>87</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J9" s="2">
         <v>41</v>
       </c>
-      <c r="K9" s="14">
+      <c r="K9" s="2">
         <v>309</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M9" s="16" t="s">
-        <v>15</v>
+        <v>27</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.78030303030303028</v>
       </c>
       <c r="N9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.86513157894736847</v>
+      </c>
+      <c r="O9" s="2">
+        <f t="shared" si="2"/>
+        <v>0.24857142857142858</v>
+      </c>
+      <c r="P9" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q9" s="2">
         <v>21</v>
       </c>
-      <c r="O9" s="2">
+      <c r="R9" s="2">
         <v>12</v>
       </c>
-      <c r="P9" s="2">
+      <c r="S9" s="2">
         <v>0</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="T9" s="2">
         <v>33</v>
       </c>
-      <c r="R9" s="2" t="s">
-        <v>17</v>
+      <c r="U9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="3"/>
+        <v>0.73333333333333328</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="5"/>
+        <v>0.36363636363636365</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
     </row>
-    <row r="11" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+    <row r="11" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>6</v>
       </c>
       <c r="B11">
         <v>4125</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11">
         <v>15</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="2">
+        <v>313</v>
+      </c>
+      <c r="I11" s="2">
+        <v>37</v>
+      </c>
+      <c r="J11" s="2">
+        <v>46</v>
+      </c>
+      <c r="K11" s="2">
+        <v>304</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.89149560117302051</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.871866295264624</v>
+      </c>
+      <c r="O11" s="2">
+        <f t="shared" si="2"/>
+        <v>0.10571428571428572</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>19</v>
+      </c>
+      <c r="R11" s="2">
         <v>14</v>
       </c>
-      <c r="G11" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="17">
-        <v>313</v>
-      </c>
-      <c r="I11" s="17">
+      <c r="S11" s="2">
+        <v>0</v>
+      </c>
+      <c r="T11" s="2">
+        <v>33</v>
+      </c>
+      <c r="U11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J11" s="17">
-        <v>46</v>
-      </c>
-      <c r="K11" s="17">
-        <v>304</v>
-      </c>
-      <c r="L11" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="M11" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="N11" s="17">
-        <v>19</v>
-      </c>
-      <c r="O11" s="17">
-        <v>14</v>
-      </c>
-      <c r="P11" s="17">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="17">
-        <v>33</v>
-      </c>
-      <c r="R11" s="17" t="s">
-        <v>16</v>
+      <c r="V11">
+        <f t="shared" si="3"/>
+        <v>0.7021276595744681</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="5"/>
+        <v>0.42424242424242425</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
+    <row r="12" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>7</v>
       </c>
       <c r="B12">
         <v>4125</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12">
         <v>15</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="H12" s="17">
+        <v>20</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="2">
         <v>310</v>
       </c>
-      <c r="I12" s="17">
+      <c r="I12" s="2">
         <v>40</v>
       </c>
-      <c r="J12" s="17">
+      <c r="J12" s="2">
         <v>46</v>
       </c>
-      <c r="K12" s="17">
+      <c r="K12" s="2">
         <v>304</v>
       </c>
-      <c r="L12" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="M12" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="N12" s="17">
+      <c r="L12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.88372093023255816</v>
+      </c>
+      <c r="N12" s="2">
+        <f t="shared" si="1"/>
+        <v>0.8707865168539326</v>
+      </c>
+      <c r="O12" s="2">
+        <f t="shared" si="2"/>
+        <v>0.11428571428571428</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q12" s="2">
         <v>21</v>
       </c>
-      <c r="O12" s="17">
+      <c r="R12" s="2">
         <v>12</v>
       </c>
-      <c r="P12" s="17">
+      <c r="S12" s="2">
         <v>1</v>
       </c>
-      <c r="Q12" s="17">
+      <c r="T12" s="2">
         <v>32</v>
       </c>
-      <c r="R12" s="17" t="s">
-        <v>40</v>
+      <c r="U12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="3"/>
+        <v>0.72727272727272729</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="4"/>
+        <v>0.95454545454545459</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="5"/>
+        <v>0.36363636363636365</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>8</v>
       </c>
@@ -1137,80 +1338,107 @@
         <v>4125</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13">
         <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" s="14">
+        <v>20</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="2">
         <v>262</v>
       </c>
-      <c r="I13" s="14">
+      <c r="I13" s="2">
         <v>88</v>
       </c>
-      <c r="J13" s="14">
+      <c r="J13" s="2">
         <v>38</v>
       </c>
-      <c r="K13" s="14">
+      <c r="K13" s="2">
         <v>312</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="M13" s="16" t="s">
-        <v>15</v>
+        <v>27</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="0"/>
+        <v>0.78</v>
       </c>
       <c r="N13" s="2">
+        <f t="shared" si="1"/>
+        <v>0.87333333333333329</v>
+      </c>
+      <c r="O13" s="2">
+        <f t="shared" si="2"/>
+        <v>0.25142857142857145</v>
+      </c>
+      <c r="P13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q13" s="2">
         <v>21</v>
       </c>
-      <c r="O13" s="2">
+      <c r="R13" s="2">
         <v>12</v>
       </c>
-      <c r="P13" s="2">
+      <c r="S13" s="2">
         <v>0</v>
       </c>
-      <c r="Q13" s="2">
+      <c r="T13" s="2">
         <v>33</v>
       </c>
-      <c r="R13" s="2" t="s">
-        <v>17</v>
+      <c r="U13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="3"/>
+        <v>0.73333333333333328</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="5"/>
+        <v>0.36363636363636365</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
+    <row r="14" spans="1:24" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="G2:L2"/>
-    <mergeCell ref="M2:R2"/>
+    <mergeCell ref="P2:U2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1486,16 +1714,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5971D2C-0C87-417B-8A36-A1DD6DD3EDDD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="db9da065-8187-44dc-ad23-3b6307f2cf84"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="39f17169-dc69-4319-88e3-df32810e06be"/>
-    <ds:schemaRef ds:uri="db9da065-8187-44dc-ad23-3b6307f2cf84"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>